<commit_message>
Delete unneccessary files and modify some steps in the pages classes
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1575622A-1B75-4F20-AAE2-9C5DCFEAC1C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296AFF7-294E-4C8D-918F-2622A6A92C9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,16 +96,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>ATestBAutomation1234567a1</t>
-  </si>
-  <si>
-    <t>Facility_A1091a1</t>
-  </si>
-  <si>
-    <t>Pharmacy_A1091a1</t>
-  </si>
-  <si>
-    <t>Alignment Project A1091a1</t>
+    <t>ATestBAutomation1234567a12</t>
+  </si>
+  <si>
+    <t>Facility_A1091a12</t>
+  </si>
+  <si>
+    <t>Pharmacy_A1091a12</t>
+  </si>
+  <si>
+    <t>Alignment Project A1091a12</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify wait in all pages classes and update TestData file records
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296AFF7-294E-4C8D-918F-2622A6A92C9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80C1986-A4A5-414C-92BA-3DA5E5AB98D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,16 +96,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>ATestBAutomation1234567a12</t>
-  </si>
-  <si>
-    <t>Facility_A1091a12</t>
-  </si>
-  <si>
-    <t>Pharmacy_A1091a12</t>
-  </si>
-  <si>
-    <t>Alignment Project A1091a12</t>
+    <t>ATestBAutomationA1</t>
+  </si>
+  <si>
+    <t>Facility_C1091a1222</t>
+  </si>
+  <si>
+    <t>Pharmacy_C1091a1222</t>
+  </si>
+  <si>
+    <t>Alignment Project C1091a1222</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="61.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
Update test data file
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80C1986-A4A5-414C-92BA-3DA5E5AB98D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D3CF0-D8C7-4990-AE75-15203DB2EFA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,16 +96,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>ATestBAutomationA1</t>
-  </si>
-  <si>
-    <t>Facility_C1091a1222</t>
-  </si>
-  <si>
-    <t>Pharmacy_C1091a1222</t>
-  </si>
-  <si>
-    <t>Alignment Project C1091a1222</t>
+    <t>ATestCAutomationA1</t>
+  </si>
+  <si>
+    <t>Facility_D1091a1222</t>
+  </si>
+  <si>
+    <t>Pharmacy_D1091a1222</t>
+  </si>
+  <si>
+    <t>Alignment Project D1091a1222</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Alignment Project page class and update the test data file with new records
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D3CF0-D8C7-4990-AE75-15203DB2EFA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47521E2F-7137-4ACF-B0DE-23EC0A3A1021}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,16 +96,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>ATestCAutomationA1</t>
-  </si>
-  <si>
-    <t>Facility_D1091a1222</t>
-  </si>
-  <si>
-    <t>Pharmacy_D1091a1222</t>
-  </si>
-  <si>
-    <t>Alignment Project D1091a1222</t>
+    <t>ATestCAutomationC1</t>
+  </si>
+  <si>
+    <t>Facility_E1091a1222</t>
+  </si>
+  <si>
+    <t>Pharmacy_E1091a1222</t>
+  </si>
+  <si>
+    <t>Alignment Project E1091a1222</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modifing the script to try different scenario
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47521E2F-7137-4ACF-B0DE-23EC0A3A1021}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7395463-853F-4580-99FD-85360F0E1D3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding different method to upload files in selenium web driver and updating Test data used in data driven
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7395463-853F-4580-99FD-85360F0E1D3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0339E46F-26FE-48AE-9504-1B33255954CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,16 +96,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>ATestCAutomationC1</t>
-  </si>
-  <si>
-    <t>Facility_E1091a1222</t>
-  </si>
-  <si>
-    <t>Pharmacy_E1091a1222</t>
-  </si>
-  <si>
-    <t>Alignment Project E1091a1222</t>
+    <t>TestAutomation_POC5</t>
+  </si>
+  <si>
+    <t>Facility_POC5</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC5</t>
+  </si>
+  <si>
+    <t>Alignment Project _POC5</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update the script and adding Firefox driver to the script
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B990C09-2120-431E-9E97-53E742488E52}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AC1314-EDD8-49ED-8506-FB720909041B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Chrome property</t>
   </si>
@@ -96,23 +96,35 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>TestAutomation179</t>
-  </si>
-  <si>
-    <t>Facility_POC179</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC179</t>
-  </si>
-  <si>
-    <t>AlignmentProjectPOC179</t>
+    <t>Firefox property</t>
+  </si>
+  <si>
+    <t>Firefox driver</t>
+  </si>
+  <si>
+    <t>.\\geckodriver.exe</t>
+  </si>
+  <si>
+    <t>webdriver.gecko.driver</t>
+  </si>
+  <si>
+    <t>TestAutomation309</t>
+  </si>
+  <si>
+    <t>Facility_POC309</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC309</t>
+  </si>
+  <si>
+    <t>AlignmentProjectPOC309</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +163,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -369,16 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -420,7 +434,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,6 +450,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -721,7 +740,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,140 +761,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="9"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="7"/>
+      <c r="F4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
+      <c r="F5" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="10"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="31" t="s">
+    <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="34"/>
+      <c r="H8" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Organize the Project Script
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\git\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B03FB1-F45D-41CA-9378-1997858E71D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF8AAA-E377-43F2-98D2-0901E15CB323}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,16 +108,16 @@
     <t>Carefusion@5</t>
   </si>
   <si>
-    <t>TestAutomation319</t>
-  </si>
-  <si>
-    <t>Facility_POC319</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC319</t>
-  </si>
-  <si>
-    <t>AlignmentProjectPOC319</t>
+    <t>TestAutomation5oct</t>
+  </si>
+  <si>
+    <t>Facility_POC5oct</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC5oct</t>
+  </si>
+  <si>
+    <t>Epic101205</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Add Capture screenshot feature to the script
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\git\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF8AAA-E377-43F2-98D2-0901E15CB323}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5C4E9C-17C7-4BF5-A7D3-3D94D2215D44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,16 +108,16 @@
     <t>Carefusion@5</t>
   </si>
   <si>
-    <t>TestAutomation5oct</t>
-  </si>
-  <si>
-    <t>Facility_POC5oct</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC5oct</t>
-  </si>
-  <si>
     <t>Epic101205</t>
+  </si>
+  <si>
+    <t>TestAutomation16oct</t>
+  </si>
+  <si>
+    <t>Facility_POC16oct</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC16oct</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,28 +879,28 @@
     </row>
     <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I8" s="31"/>
     </row>

</xml_diff>

<commit_message>
Update test date Update login credentials Modify test script due to changes ocurred in stage A server
</commit_message>
<xml_diff>
--- a/SeleniumWithJava/TestData/TestData1.xlsx
+++ b/SeleniumWithJava/TestData/TestData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\git\Selenium-Java\SeleniumWithJava\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5C4E9C-17C7-4BF5-A7D3-3D94D2215D44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485F031F-E1D6-4867-9048-97456D823C8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Chrome property</t>
   </si>
@@ -102,22 +102,22 @@
     <t>webdriver.gecko.driver</t>
   </si>
   <si>
-    <t>Rola.khalaf2@bd.com</t>
-  </si>
-  <si>
-    <t>Carefusion@5</t>
-  </si>
-  <si>
     <t>Epic101205</t>
   </si>
   <si>
-    <t>TestAutomation16oct</t>
-  </si>
-  <si>
     <t>Facility_POC16oct</t>
   </si>
   <si>
     <t>Pharmacy_POC16oct</t>
+  </si>
+  <si>
+    <t>ahmed.mohamed@bd.com</t>
+  </si>
+  <si>
+    <t>WqCi119B</t>
+  </si>
+  <si>
+    <t>TestAutomation4112019</t>
   </si>
 </sst>
 </file>
@@ -740,45 +740,45 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="61.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="61.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -789,7 +789,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -814,7 +814,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
@@ -839,7 +839,7 @@
       <c r="H5" s="24"/>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -850,7 +850,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -877,36 +877,36 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="27">
+        <v>4112019</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="28">
+        <v>41120190</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{6D4D7268-FF36-4147-AC89-D50152B02129}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Carefusion@5" xr:uid="{6D4D7268-FF36-4147-AC89-D50152B02129}"/>
     <hyperlink ref="B1" r:id="rId2" xr:uid="{D2B64076-9C8E-4BBE-8417-6B9C97147497}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>